<commit_message>
tissue DB fixes mostly
</commit_message>
<xml_diff>
--- a/Lookup_table_spreadsheets/sln_tissue__Antibody.xlsx
+++ b/Lookup_table_spreadsheets/sln_tissue__Antibody.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregschwartz/matlab/DJ_schwartzlab/Lookup_table_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C002F63B-6139-8D4F-838A-70332AEED497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2F6A19-38A5-434F-8271-931EC494C6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18120" yWindow="4800" windowWidth="41400" windowHeight="23040" xr2:uid="{5919FF99-B054-5E49-89C1-0F21ABB6D4A1}"/>
+    <workbookView xWindow="13860" yWindow="4440" windowWidth="41400" windowHeight="23040" xr2:uid="{5919FF99-B054-5E49-89C1-0F21ABB6D4A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1398,8 +1398,8 @@
   </sheetPr>
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>